<commit_message>
BE Actors TimeSheet Exporrt : Generate Monthly WorkHour Report (WIP : add monthly figures (hours, extra hours)
</commit_message>
<xml_diff>
--- a/Ressources/DocTemplates/ATTACHEMENT _REF_CITY.xlsx
+++ b/Ressources/DocTemplates/ATTACHEMENT _REF_CITY.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laurent\Golang\src\github.com\lpuig\ewin\doe\Ressources\DocTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D367C531-DACB-4BE7-BA31-AC749C6262E0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B35CE99-54C6-42A8-A44F-A424D2DF61CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3945" yWindow="9870" windowWidth="28770" windowHeight="15570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2385" yWindow="1665" windowWidth="38250" windowHeight="27915" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EWIN" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -240,7 +241,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -422,11 +423,13 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="hair">
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -435,10 +438,40 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -451,7 +484,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -474,9 +507,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -504,18 +534,9 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -525,7 +546,7 @@
     <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -533,6 +554,51 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -671,7 +737,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>156883</xdr:colOff>
+      <xdr:colOff>369155</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>93655</xdr:rowOff>
     </xdr:to>
@@ -980,21 +1046,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:N190"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="175" zoomScaleNormal="100" zoomScaleSheetLayoutView="175" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.140625" customWidth="1"/>
+    <col min="3" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="34" customWidth="1"/>
     <col min="7" max="7" width="17.28515625" customWidth="1"/>
     <col min="8" max="8" width="12.85546875" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:14">
@@ -1059,1081 +1124,1073 @@
       <c r="N10" s="8"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="35"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="36"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="47"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="15" t="s">
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="J12" s="15" t="s">
+      <c r="J12" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="K12" s="16" t="s">
+      <c r="K12" s="15" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="1">
-        <v>75</v>
-      </c>
-      <c r="J13" s="24">
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="21">
         <f>SUMIF($E$21:$E$220,B13,$H$21:$H$220)</f>
         <v>0</v>
       </c>
-      <c r="K13" s="17">
+      <c r="K13" s="16">
         <f t="shared" ref="K13:K16" si="0">I13*J13</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="33" t="s">
+      <c r="C14" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="1">
-        <v>50</v>
-      </c>
-      <c r="J14" s="24">
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="21">
         <f t="shared" ref="J14:J16" si="1">SUMIF($E$21:$E$220,B14,$H$21:$H$220)</f>
         <v>0</v>
       </c>
-      <c r="K14" s="17">
+      <c r="K14" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="15" customHeight="1">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="33" t="s">
+      <c r="C15" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="1">
-        <v>70</v>
-      </c>
-      <c r="J15" s="24">
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="21">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K15" s="17">
+      <c r="K15" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="15" customHeight="1">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="32" t="s">
+      <c r="C16" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="2">
-        <v>70</v>
-      </c>
-      <c r="J16" s="28">
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="24">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K16" s="29">
+      <c r="K16" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:11">
-      <c r="J17" s="18" t="s">
+      <c r="J17" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="K17" s="19">
+      <c r="K17" s="18">
         <f>SUM(K13:K16)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="30">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="D20" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="20" t="s">
+      <c r="E20" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F20" s="20" t="s">
+      <c r="F20" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="G20" s="20" t="s">
+      <c r="G20" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="H20" s="20" t="s">
+      <c r="H20" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="I20" s="20" t="s">
+      <c r="I20" s="19" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="21"/>
+      <c r="A21" s="28"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="32"/>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="21"/>
+      <c r="A22" s="33"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="37"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="21"/>
+      <c r="A23" s="33"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="37"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="21"/>
+      <c r="A24" s="33"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="37"/>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="21"/>
+      <c r="A25" s="33"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="37"/>
     </row>
     <row r="26" spans="1:11">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="21"/>
+      <c r="A26" s="33"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="37"/>
     </row>
     <row r="27" spans="1:11">
-      <c r="A27" s="10"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="21"/>
+      <c r="A27" s="33"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="37"/>
     </row>
     <row r="28" spans="1:11">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="21"/>
+      <c r="A28" s="33"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="37"/>
     </row>
     <row r="29" spans="1:11">
-      <c r="A29" s="10"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="21"/>
+      <c r="A29" s="33"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="37"/>
     </row>
     <row r="30" spans="1:11">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="21"/>
+      <c r="A30" s="33"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="37"/>
     </row>
     <row r="31" spans="1:11">
-      <c r="A31" s="10"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="21"/>
+      <c r="A31" s="33"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="36"/>
+      <c r="I31" s="37"/>
     </row>
     <row r="32" spans="1:11">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="21"/>
+      <c r="A32" s="33"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="34"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="36"/>
+      <c r="I32" s="37"/>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="10"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="21"/>
+      <c r="A33" s="33"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="36"/>
+      <c r="I33" s="37"/>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="10"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="21"/>
+      <c r="A34" s="33"/>
+      <c r="B34" s="33"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="33"/>
+      <c r="H34" s="36"/>
+      <c r="I34" s="37"/>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="10"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="21"/>
+      <c r="A35" s="33"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="33"/>
+      <c r="H35" s="36"/>
+      <c r="I35" s="37"/>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="10"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="21"/>
+      <c r="A36" s="33"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="35"/>
+      <c r="G36" s="33"/>
+      <c r="H36" s="36"/>
+      <c r="I36" s="37"/>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="10"/>
-      <c r="B37" s="10"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="21"/>
+      <c r="A37" s="33"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="33"/>
+      <c r="F37" s="35"/>
+      <c r="G37" s="33"/>
+      <c r="H37" s="36"/>
+      <c r="I37" s="37"/>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="10"/>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="21"/>
+      <c r="A38" s="33"/>
+      <c r="B38" s="33"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="33"/>
+      <c r="F38" s="35"/>
+      <c r="G38" s="33"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="37"/>
     </row>
     <row r="39" spans="1:9">
-      <c r="A39" s="9"/>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="21"/>
+      <c r="A39" s="33"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="35"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="36"/>
+      <c r="I39" s="37"/>
     </row>
     <row r="40" spans="1:9">
-      <c r="A40" s="9"/>
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="21"/>
+      <c r="A40" s="33"/>
+      <c r="B40" s="33"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="36"/>
+      <c r="I40" s="37"/>
     </row>
     <row r="41" spans="1:9">
-      <c r="A41" s="9"/>
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="11"/>
-      <c r="I41" s="21"/>
+      <c r="A41" s="33"/>
+      <c r="B41" s="33"/>
+      <c r="C41" s="34"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="35"/>
+      <c r="G41" s="33"/>
+      <c r="H41" s="36"/>
+      <c r="I41" s="37"/>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" s="9"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="11"/>
-      <c r="I42" s="21"/>
+      <c r="A42" s="33"/>
+      <c r="B42" s="33"/>
+      <c r="C42" s="34"/>
+      <c r="D42" s="34"/>
+      <c r="E42" s="33"/>
+      <c r="F42" s="35"/>
+      <c r="G42" s="33"/>
+      <c r="H42" s="36"/>
+      <c r="I42" s="37"/>
     </row>
     <row r="43" spans="1:9">
-      <c r="A43" s="9"/>
-      <c r="B43" s="9"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="11"/>
-      <c r="I43" s="21"/>
+      <c r="A43" s="33"/>
+      <c r="B43" s="33"/>
+      <c r="C43" s="34"/>
+      <c r="D43" s="34"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="35"/>
+      <c r="G43" s="33"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="37"/>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="9"/>
-      <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="11"/>
-      <c r="I44" s="21"/>
+      <c r="A44" s="33"/>
+      <c r="B44" s="33"/>
+      <c r="C44" s="34"/>
+      <c r="D44" s="34"/>
+      <c r="E44" s="33"/>
+      <c r="F44" s="35"/>
+      <c r="G44" s="33"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="37"/>
     </row>
     <row r="45" spans="1:9">
-      <c r="A45" s="9"/>
-      <c r="B45" s="9"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="21"/>
+      <c r="A45" s="33"/>
+      <c r="B45" s="33"/>
+      <c r="C45" s="34"/>
+      <c r="D45" s="34"/>
+      <c r="E45" s="33"/>
+      <c r="F45" s="35"/>
+      <c r="G45" s="33"/>
+      <c r="H45" s="36"/>
+      <c r="I45" s="37"/>
     </row>
     <row r="46" spans="1:9">
-      <c r="A46" s="9"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="10"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="11"/>
-      <c r="I46" s="21"/>
+      <c r="A46" s="33"/>
+      <c r="B46" s="33"/>
+      <c r="C46" s="34"/>
+      <c r="D46" s="34"/>
+      <c r="E46" s="33"/>
+      <c r="F46" s="35"/>
+      <c r="G46" s="33"/>
+      <c r="H46" s="36"/>
+      <c r="I46" s="37"/>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="9"/>
-      <c r="B47" s="9"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="9"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="21"/>
+      <c r="A47" s="33"/>
+      <c r="B47" s="33"/>
+      <c r="C47" s="34"/>
+      <c r="D47" s="34"/>
+      <c r="E47" s="33"/>
+      <c r="F47" s="35"/>
+      <c r="G47" s="33"/>
+      <c r="H47" s="36"/>
+      <c r="I47" s="37"/>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="9"/>
-      <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="10"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="12"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="21"/>
+      <c r="A48" s="33"/>
+      <c r="B48" s="33"/>
+      <c r="C48" s="34"/>
+      <c r="D48" s="34"/>
+      <c r="E48" s="33"/>
+      <c r="F48" s="35"/>
+      <c r="G48" s="33"/>
+      <c r="H48" s="36"/>
+      <c r="I48" s="37"/>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="9"/>
-      <c r="B49" s="9"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="12"/>
-      <c r="H49" s="11"/>
-      <c r="I49" s="21"/>
+      <c r="A49" s="33"/>
+      <c r="B49" s="33"/>
+      <c r="C49" s="34"/>
+      <c r="D49" s="34"/>
+      <c r="E49" s="33"/>
+      <c r="F49" s="35"/>
+      <c r="G49" s="33"/>
+      <c r="H49" s="36"/>
+      <c r="I49" s="37"/>
     </row>
     <row r="50" spans="1:9">
-      <c r="A50" s="9"/>
-      <c r="B50" s="9"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="12"/>
-      <c r="H50" s="11"/>
-      <c r="I50" s="21"/>
+      <c r="A50" s="33"/>
+      <c r="B50" s="33"/>
+      <c r="C50" s="34"/>
+      <c r="D50" s="34"/>
+      <c r="E50" s="33"/>
+      <c r="F50" s="35"/>
+      <c r="G50" s="33"/>
+      <c r="H50" s="36"/>
+      <c r="I50" s="37"/>
     </row>
     <row r="51" spans="1:9">
-      <c r="A51" s="9"/>
-      <c r="B51" s="9"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="10"/>
-      <c r="H51" s="11"/>
-      <c r="I51" s="21"/>
+      <c r="A51" s="33"/>
+      <c r="B51" s="33"/>
+      <c r="C51" s="34"/>
+      <c r="D51" s="34"/>
+      <c r="E51" s="33"/>
+      <c r="F51" s="35"/>
+      <c r="G51" s="33"/>
+      <c r="H51" s="36"/>
+      <c r="I51" s="37"/>
     </row>
     <row r="52" spans="1:9">
-      <c r="A52" s="9"/>
-      <c r="B52" s="9"/>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="10"/>
-      <c r="H52" s="11"/>
-      <c r="I52" s="21"/>
+      <c r="A52" s="33"/>
+      <c r="B52" s="33"/>
+      <c r="C52" s="34"/>
+      <c r="D52" s="34"/>
+      <c r="E52" s="33"/>
+      <c r="F52" s="35"/>
+      <c r="G52" s="33"/>
+      <c r="H52" s="36"/>
+      <c r="I52" s="37"/>
     </row>
     <row r="53" spans="1:9">
-      <c r="A53" s="9"/>
-      <c r="B53" s="9"/>
-      <c r="C53" s="9"/>
-      <c r="D53" s="9"/>
-      <c r="E53" s="10"/>
-      <c r="F53" s="9"/>
-      <c r="G53" s="10"/>
-      <c r="H53" s="11"/>
-      <c r="I53" s="21"/>
+      <c r="A53" s="33"/>
+      <c r="B53" s="33"/>
+      <c r="C53" s="34"/>
+      <c r="D53" s="34"/>
+      <c r="E53" s="33"/>
+      <c r="F53" s="35"/>
+      <c r="G53" s="33"/>
+      <c r="H53" s="36"/>
+      <c r="I53" s="37"/>
     </row>
     <row r="54" spans="1:9">
-      <c r="A54" s="9"/>
-      <c r="B54" s="9"/>
-      <c r="C54" s="9"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="10"/>
-      <c r="F54" s="9"/>
-      <c r="G54" s="10"/>
-      <c r="H54" s="11"/>
-      <c r="I54" s="21"/>
+      <c r="A54" s="33"/>
+      <c r="B54" s="33"/>
+      <c r="C54" s="34"/>
+      <c r="D54" s="34"/>
+      <c r="E54" s="33"/>
+      <c r="F54" s="35"/>
+      <c r="G54" s="33"/>
+      <c r="H54" s="36"/>
+      <c r="I54" s="37"/>
     </row>
     <row r="55" spans="1:9">
-      <c r="A55" s="9"/>
-      <c r="B55" s="9"/>
-      <c r="C55" s="9"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="10"/>
-      <c r="F55" s="9"/>
-      <c r="G55" s="10"/>
-      <c r="H55" s="11"/>
-      <c r="I55" s="21"/>
+      <c r="A55" s="33"/>
+      <c r="B55" s="33"/>
+      <c r="C55" s="34"/>
+      <c r="D55" s="34"/>
+      <c r="E55" s="33"/>
+      <c r="F55" s="35"/>
+      <c r="G55" s="33"/>
+      <c r="H55" s="36"/>
+      <c r="I55" s="37"/>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" s="9"/>
-      <c r="B56" s="9"/>
-      <c r="C56" s="9"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="10"/>
-      <c r="F56" s="9"/>
-      <c r="G56" s="10"/>
-      <c r="H56" s="11"/>
-      <c r="I56" s="21"/>
+      <c r="A56" s="33"/>
+      <c r="B56" s="33"/>
+      <c r="C56" s="34"/>
+      <c r="D56" s="34"/>
+      <c r="E56" s="33"/>
+      <c r="F56" s="35"/>
+      <c r="G56" s="33"/>
+      <c r="H56" s="36"/>
+      <c r="I56" s="37"/>
     </row>
     <row r="57" spans="1:9">
-      <c r="A57" s="9"/>
-      <c r="B57" s="9"/>
-      <c r="C57" s="9"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="10"/>
-      <c r="F57" s="9"/>
-      <c r="G57" s="10"/>
-      <c r="H57" s="11"/>
-      <c r="I57" s="21"/>
+      <c r="A57" s="33"/>
+      <c r="B57" s="33"/>
+      <c r="C57" s="34"/>
+      <c r="D57" s="34"/>
+      <c r="E57" s="33"/>
+      <c r="F57" s="35"/>
+      <c r="G57" s="33"/>
+      <c r="H57" s="36"/>
+      <c r="I57" s="37"/>
     </row>
     <row r="58" spans="1:9">
-      <c r="A58" s="9"/>
-      <c r="B58" s="9"/>
-      <c r="C58" s="9"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="10"/>
-      <c r="F58" s="9"/>
-      <c r="G58" s="9"/>
-      <c r="H58" s="11"/>
-      <c r="I58" s="21"/>
+      <c r="A58" s="33"/>
+      <c r="B58" s="33"/>
+      <c r="C58" s="34"/>
+      <c r="D58" s="34"/>
+      <c r="E58" s="33"/>
+      <c r="F58" s="35"/>
+      <c r="G58" s="33"/>
+      <c r="H58" s="36"/>
+      <c r="I58" s="37"/>
     </row>
     <row r="59" spans="1:9">
-      <c r="A59" s="9"/>
-      <c r="B59" s="9"/>
-      <c r="C59" s="9"/>
-      <c r="D59" s="9"/>
-      <c r="E59" s="10"/>
-      <c r="F59" s="9"/>
-      <c r="G59" s="9"/>
-      <c r="H59" s="11"/>
-      <c r="I59" s="21"/>
+      <c r="A59" s="33"/>
+      <c r="B59" s="33"/>
+      <c r="C59" s="34"/>
+      <c r="D59" s="34"/>
+      <c r="E59" s="33"/>
+      <c r="F59" s="35"/>
+      <c r="G59" s="33"/>
+      <c r="H59" s="36"/>
+      <c r="I59" s="37"/>
     </row>
     <row r="60" spans="1:9">
-      <c r="A60" s="9"/>
-      <c r="B60" s="9"/>
-      <c r="C60" s="9"/>
-      <c r="D60" s="9"/>
-      <c r="E60" s="10"/>
-      <c r="F60" s="9"/>
-      <c r="G60" s="9"/>
-      <c r="H60" s="11"/>
-      <c r="I60" s="21"/>
+      <c r="A60" s="33"/>
+      <c r="B60" s="33"/>
+      <c r="C60" s="34"/>
+      <c r="D60" s="34"/>
+      <c r="E60" s="33"/>
+      <c r="F60" s="35"/>
+      <c r="G60" s="33"/>
+      <c r="H60" s="36"/>
+      <c r="I60" s="37"/>
     </row>
     <row r="61" spans="1:9">
-      <c r="A61" s="9"/>
-      <c r="B61" s="9"/>
-      <c r="C61" s="9"/>
-      <c r="D61" s="9"/>
-      <c r="E61" s="10"/>
-      <c r="F61" s="9"/>
-      <c r="G61" s="9"/>
-      <c r="H61" s="11"/>
-      <c r="I61" s="21"/>
+      <c r="A61" s="33"/>
+      <c r="B61" s="33"/>
+      <c r="C61" s="34"/>
+      <c r="D61" s="34"/>
+      <c r="E61" s="33"/>
+      <c r="F61" s="35"/>
+      <c r="G61" s="33"/>
+      <c r="H61" s="36"/>
+      <c r="I61" s="37"/>
     </row>
     <row r="62" spans="1:9">
-      <c r="A62" s="9"/>
-      <c r="B62" s="9"/>
-      <c r="C62" s="9"/>
-      <c r="D62" s="9"/>
-      <c r="E62" s="10"/>
-      <c r="F62" s="9"/>
-      <c r="G62" s="9"/>
-      <c r="H62" s="11"/>
-      <c r="I62" s="21"/>
+      <c r="A62" s="33"/>
+      <c r="B62" s="33"/>
+      <c r="C62" s="34"/>
+      <c r="D62" s="34"/>
+      <c r="E62" s="33"/>
+      <c r="F62" s="35"/>
+      <c r="G62" s="33"/>
+      <c r="H62" s="36"/>
+      <c r="I62" s="37"/>
     </row>
     <row r="63" spans="1:9">
-      <c r="A63" s="9"/>
-      <c r="B63" s="9"/>
-      <c r="C63" s="9"/>
-      <c r="D63" s="9"/>
-      <c r="E63" s="10"/>
-      <c r="F63" s="9"/>
-      <c r="G63" s="9"/>
-      <c r="H63" s="11"/>
-      <c r="I63" s="21"/>
+      <c r="A63" s="33"/>
+      <c r="B63" s="33"/>
+      <c r="C63" s="34"/>
+      <c r="D63" s="34"/>
+      <c r="E63" s="33"/>
+      <c r="F63" s="35"/>
+      <c r="G63" s="33"/>
+      <c r="H63" s="36"/>
+      <c r="I63" s="37"/>
     </row>
     <row r="64" spans="1:9">
-      <c r="A64" s="9"/>
-      <c r="B64" s="9"/>
-      <c r="C64" s="9"/>
-      <c r="D64" s="9"/>
-      <c r="E64" s="10"/>
-      <c r="F64" s="9"/>
-      <c r="G64" s="9"/>
-      <c r="H64" s="11"/>
-      <c r="I64" s="21"/>
+      <c r="A64" s="33"/>
+      <c r="B64" s="33"/>
+      <c r="C64" s="34"/>
+      <c r="D64" s="34"/>
+      <c r="E64" s="33"/>
+      <c r="F64" s="35"/>
+      <c r="G64" s="33"/>
+      <c r="H64" s="36"/>
+      <c r="I64" s="37"/>
     </row>
     <row r="65" spans="1:9">
-      <c r="A65" s="9"/>
-      <c r="B65" s="9"/>
-      <c r="C65" s="9"/>
-      <c r="D65" s="9"/>
-      <c r="E65" s="10"/>
-      <c r="F65" s="9"/>
-      <c r="G65" s="9"/>
-      <c r="H65" s="11"/>
-      <c r="I65" s="21"/>
+      <c r="A65" s="33"/>
+      <c r="B65" s="33"/>
+      <c r="C65" s="34"/>
+      <c r="D65" s="34"/>
+      <c r="E65" s="33"/>
+      <c r="F65" s="35"/>
+      <c r="G65" s="33"/>
+      <c r="H65" s="36"/>
+      <c r="I65" s="37"/>
     </row>
     <row r="66" spans="1:9">
-      <c r="A66" s="9"/>
-      <c r="B66" s="9"/>
-      <c r="C66" s="9"/>
-      <c r="D66" s="9"/>
-      <c r="E66" s="10"/>
-      <c r="F66" s="9"/>
-      <c r="G66" s="9"/>
-      <c r="H66" s="11"/>
-      <c r="I66" s="21"/>
+      <c r="A66" s="33"/>
+      <c r="B66" s="33"/>
+      <c r="C66" s="34"/>
+      <c r="D66" s="34"/>
+      <c r="E66" s="33"/>
+      <c r="F66" s="35"/>
+      <c r="G66" s="33"/>
+      <c r="H66" s="36"/>
+      <c r="I66" s="37"/>
     </row>
     <row r="67" spans="1:9">
-      <c r="A67" s="9"/>
-      <c r="B67" s="9"/>
-      <c r="C67" s="9"/>
-      <c r="D67" s="9"/>
-      <c r="E67" s="10"/>
-      <c r="F67" s="9"/>
-      <c r="G67" s="9"/>
-      <c r="H67" s="11"/>
-      <c r="I67" s="21"/>
+      <c r="A67" s="33"/>
+      <c r="B67" s="33"/>
+      <c r="C67" s="34"/>
+      <c r="D67" s="34"/>
+      <c r="E67" s="33"/>
+      <c r="F67" s="35"/>
+      <c r="G67" s="33"/>
+      <c r="H67" s="36"/>
+      <c r="I67" s="37"/>
     </row>
     <row r="68" spans="1:9">
-      <c r="A68" s="9"/>
-      <c r="B68" s="9"/>
-      <c r="C68" s="9"/>
-      <c r="D68" s="9"/>
-      <c r="E68" s="10"/>
-      <c r="F68" s="9"/>
-      <c r="G68" s="9"/>
-      <c r="H68" s="11"/>
-      <c r="I68" s="21"/>
+      <c r="A68" s="33"/>
+      <c r="B68" s="33"/>
+      <c r="C68" s="34"/>
+      <c r="D68" s="34"/>
+      <c r="E68" s="33"/>
+      <c r="F68" s="35"/>
+      <c r="G68" s="33"/>
+      <c r="H68" s="36"/>
+      <c r="I68" s="37"/>
     </row>
     <row r="69" spans="1:9">
-      <c r="A69" s="9"/>
-      <c r="B69" s="9"/>
-      <c r="C69" s="9"/>
-      <c r="D69" s="9"/>
-      <c r="E69" s="10"/>
-      <c r="F69" s="9"/>
-      <c r="G69" s="9"/>
-      <c r="H69" s="11"/>
-      <c r="I69" s="21"/>
+      <c r="A69" s="33"/>
+      <c r="B69" s="33"/>
+      <c r="C69" s="34"/>
+      <c r="D69" s="34"/>
+      <c r="E69" s="33"/>
+      <c r="F69" s="35"/>
+      <c r="G69" s="33"/>
+      <c r="H69" s="36"/>
+      <c r="I69" s="37"/>
     </row>
     <row r="70" spans="1:9">
-      <c r="A70" s="9"/>
-      <c r="B70" s="9"/>
-      <c r="C70" s="9"/>
-      <c r="D70" s="9"/>
-      <c r="E70" s="10"/>
-      <c r="F70" s="9"/>
-      <c r="G70" s="9"/>
-      <c r="H70" s="11"/>
-      <c r="I70" s="21"/>
+      <c r="A70" s="33"/>
+      <c r="B70" s="33"/>
+      <c r="C70" s="34"/>
+      <c r="D70" s="34"/>
+      <c r="E70" s="33"/>
+      <c r="F70" s="35"/>
+      <c r="G70" s="33"/>
+      <c r="H70" s="36"/>
+      <c r="I70" s="37"/>
     </row>
     <row r="71" spans="1:9">
-      <c r="A71" s="9"/>
-      <c r="B71" s="9"/>
-      <c r="C71" s="9"/>
-      <c r="D71" s="9"/>
-      <c r="E71" s="10"/>
-      <c r="F71" s="9"/>
-      <c r="G71" s="9"/>
-      <c r="H71" s="11"/>
-      <c r="I71" s="21"/>
+      <c r="A71" s="33"/>
+      <c r="B71" s="33"/>
+      <c r="C71" s="34"/>
+      <c r="D71" s="34"/>
+      <c r="E71" s="33"/>
+      <c r="F71" s="35"/>
+      <c r="G71" s="33"/>
+      <c r="H71" s="36"/>
+      <c r="I71" s="37"/>
     </row>
     <row r="72" spans="1:9">
-      <c r="A72" s="9"/>
-      <c r="B72" s="9"/>
-      <c r="C72" s="9"/>
-      <c r="D72" s="9"/>
-      <c r="E72" s="10"/>
-      <c r="F72" s="9"/>
-      <c r="G72" s="9"/>
-      <c r="H72" s="11"/>
-      <c r="I72" s="21"/>
+      <c r="A72" s="33"/>
+      <c r="B72" s="33"/>
+      <c r="C72" s="34"/>
+      <c r="D72" s="34"/>
+      <c r="E72" s="33"/>
+      <c r="F72" s="35"/>
+      <c r="G72" s="33"/>
+      <c r="H72" s="36"/>
+      <c r="I72" s="37"/>
     </row>
     <row r="73" spans="1:9">
-      <c r="A73" s="9"/>
-      <c r="B73" s="9"/>
-      <c r="C73" s="9"/>
-      <c r="D73" s="9"/>
-      <c r="E73" s="10"/>
-      <c r="F73" s="9"/>
-      <c r="G73" s="9"/>
-      <c r="H73" s="11"/>
-      <c r="I73" s="21"/>
+      <c r="A73" s="33"/>
+      <c r="B73" s="33"/>
+      <c r="C73" s="34"/>
+      <c r="D73" s="34"/>
+      <c r="E73" s="33"/>
+      <c r="F73" s="35"/>
+      <c r="G73" s="33"/>
+      <c r="H73" s="36"/>
+      <c r="I73" s="37"/>
     </row>
     <row r="74" spans="1:9">
-      <c r="A74" s="9"/>
-      <c r="B74" s="9"/>
-      <c r="C74" s="9"/>
-      <c r="D74" s="9"/>
-      <c r="E74" s="10"/>
-      <c r="F74" s="9"/>
-      <c r="G74" s="9"/>
-      <c r="H74" s="11"/>
-      <c r="I74" s="21"/>
+      <c r="A74" s="33"/>
+      <c r="B74" s="33"/>
+      <c r="C74" s="34"/>
+      <c r="D74" s="34"/>
+      <c r="E74" s="33"/>
+      <c r="F74" s="35"/>
+      <c r="G74" s="33"/>
+      <c r="H74" s="36"/>
+      <c r="I74" s="37"/>
     </row>
     <row r="75" spans="1:9">
-      <c r="A75" s="9"/>
-      <c r="B75" s="9"/>
-      <c r="C75" s="9"/>
-      <c r="D75" s="9"/>
-      <c r="E75" s="10"/>
-      <c r="F75" s="9"/>
-      <c r="G75" s="9"/>
-      <c r="H75" s="11"/>
-      <c r="I75" s="21"/>
+      <c r="A75" s="33"/>
+      <c r="B75" s="33"/>
+      <c r="C75" s="34"/>
+      <c r="D75" s="34"/>
+      <c r="E75" s="33"/>
+      <c r="F75" s="35"/>
+      <c r="G75" s="33"/>
+      <c r="H75" s="36"/>
+      <c r="I75" s="37"/>
     </row>
     <row r="76" spans="1:9">
-      <c r="A76" s="9"/>
-      <c r="B76" s="9"/>
-      <c r="C76" s="9"/>
-      <c r="D76" s="9"/>
-      <c r="E76" s="10"/>
-      <c r="F76" s="9"/>
-      <c r="G76" s="9"/>
-      <c r="H76" s="11"/>
-      <c r="I76" s="21"/>
+      <c r="A76" s="33"/>
+      <c r="B76" s="33"/>
+      <c r="C76" s="34"/>
+      <c r="D76" s="34"/>
+      <c r="E76" s="33"/>
+      <c r="F76" s="35"/>
+      <c r="G76" s="33"/>
+      <c r="H76" s="36"/>
+      <c r="I76" s="37"/>
     </row>
     <row r="77" spans="1:9">
-      <c r="A77" s="9"/>
-      <c r="B77" s="9"/>
-      <c r="C77" s="9"/>
-      <c r="D77" s="9"/>
-      <c r="E77" s="10"/>
-      <c r="F77" s="9"/>
-      <c r="G77" s="9"/>
-      <c r="H77" s="11"/>
-      <c r="I77" s="21"/>
+      <c r="A77" s="33"/>
+      <c r="B77" s="33"/>
+      <c r="C77" s="34"/>
+      <c r="D77" s="34"/>
+      <c r="E77" s="33"/>
+      <c r="F77" s="35"/>
+      <c r="G77" s="33"/>
+      <c r="H77" s="36"/>
+      <c r="I77" s="37"/>
     </row>
     <row r="78" spans="1:9">
-      <c r="A78" s="9"/>
-      <c r="B78" s="9"/>
-      <c r="C78" s="9"/>
-      <c r="D78" s="9"/>
-      <c r="E78" s="10"/>
-      <c r="F78" s="9"/>
-      <c r="G78" s="9"/>
-      <c r="H78" s="11"/>
-      <c r="I78" s="21"/>
+      <c r="A78" s="33"/>
+      <c r="B78" s="33"/>
+      <c r="C78" s="34"/>
+      <c r="D78" s="34"/>
+      <c r="E78" s="33"/>
+      <c r="F78" s="35"/>
+      <c r="G78" s="33"/>
+      <c r="H78" s="36"/>
+      <c r="I78" s="37"/>
     </row>
     <row r="79" spans="1:9">
-      <c r="A79" s="9"/>
-      <c r="B79" s="9"/>
-      <c r="C79" s="9"/>
-      <c r="D79" s="9"/>
-      <c r="E79" s="10"/>
-      <c r="F79" s="9"/>
-      <c r="G79" s="9"/>
-      <c r="H79" s="11"/>
-      <c r="I79" s="21"/>
+      <c r="A79" s="33"/>
+      <c r="B79" s="33"/>
+      <c r="C79" s="34"/>
+      <c r="D79" s="34"/>
+      <c r="E79" s="33"/>
+      <c r="F79" s="35"/>
+      <c r="G79" s="33"/>
+      <c r="H79" s="36"/>
+      <c r="I79" s="37"/>
     </row>
     <row r="80" spans="1:9">
-      <c r="A80" s="9"/>
-      <c r="B80" s="9"/>
-      <c r="C80" s="9"/>
-      <c r="D80" s="9"/>
-      <c r="E80" s="10"/>
-      <c r="F80" s="9"/>
-      <c r="G80" s="9"/>
-      <c r="H80" s="11"/>
-      <c r="I80" s="21"/>
+      <c r="A80" s="33"/>
+      <c r="B80" s="33"/>
+      <c r="C80" s="34"/>
+      <c r="D80" s="34"/>
+      <c r="E80" s="33"/>
+      <c r="F80" s="35"/>
+      <c r="G80" s="33"/>
+      <c r="H80" s="36"/>
+      <c r="I80" s="37"/>
     </row>
     <row r="81" spans="1:9">
-      <c r="A81" s="9"/>
-      <c r="B81" s="9"/>
-      <c r="C81" s="9"/>
-      <c r="D81" s="9"/>
-      <c r="E81" s="10"/>
-      <c r="F81" s="9"/>
-      <c r="G81" s="9"/>
-      <c r="H81" s="11"/>
-      <c r="I81" s="21"/>
+      <c r="A81" s="33"/>
+      <c r="B81" s="33"/>
+      <c r="C81" s="34"/>
+      <c r="D81" s="34"/>
+      <c r="E81" s="33"/>
+      <c r="F81" s="35"/>
+      <c r="G81" s="33"/>
+      <c r="H81" s="36"/>
+      <c r="I81" s="37"/>
     </row>
     <row r="82" spans="1:9">
-      <c r="A82" s="9"/>
-      <c r="B82" s="9"/>
-      <c r="C82" s="9"/>
-      <c r="D82" s="9"/>
-      <c r="E82" s="10"/>
-      <c r="F82" s="9"/>
-      <c r="G82" s="9"/>
-      <c r="H82" s="11"/>
-      <c r="I82" s="21"/>
+      <c r="A82" s="33"/>
+      <c r="B82" s="33"/>
+      <c r="C82" s="34"/>
+      <c r="D82" s="34"/>
+      <c r="E82" s="33"/>
+      <c r="F82" s="35"/>
+      <c r="G82" s="33"/>
+      <c r="H82" s="36"/>
+      <c r="I82" s="37"/>
     </row>
     <row r="83" spans="1:9">
-      <c r="A83" s="9"/>
-      <c r="B83" s="9"/>
-      <c r="C83" s="9"/>
-      <c r="D83" s="9"/>
-      <c r="E83" s="10"/>
-      <c r="F83" s="9"/>
-      <c r="G83" s="9"/>
-      <c r="H83" s="11"/>
-      <c r="I83" s="21"/>
+      <c r="A83" s="33"/>
+      <c r="B83" s="33"/>
+      <c r="C83" s="34"/>
+      <c r="D83" s="34"/>
+      <c r="E83" s="33"/>
+      <c r="F83" s="35"/>
+      <c r="G83" s="33"/>
+      <c r="H83" s="36"/>
+      <c r="I83" s="37"/>
     </row>
     <row r="84" spans="1:9">
-      <c r="A84" s="9"/>
-      <c r="B84" s="9"/>
-      <c r="C84" s="9"/>
-      <c r="D84" s="9"/>
-      <c r="E84" s="10"/>
-      <c r="F84" s="9"/>
-      <c r="G84" s="9"/>
-      <c r="H84" s="11"/>
-      <c r="I84" s="21"/>
+      <c r="A84" s="33"/>
+      <c r="B84" s="33"/>
+      <c r="C84" s="34"/>
+      <c r="D84" s="34"/>
+      <c r="E84" s="33"/>
+      <c r="F84" s="35"/>
+      <c r="G84" s="33"/>
+      <c r="H84" s="36"/>
+      <c r="I84" s="37"/>
     </row>
     <row r="85" spans="1:9">
-      <c r="A85" s="9"/>
-      <c r="B85" s="9"/>
-      <c r="C85" s="9"/>
-      <c r="D85" s="9"/>
-      <c r="E85" s="10"/>
-      <c r="F85" s="9"/>
-      <c r="G85" s="9"/>
-      <c r="H85" s="11"/>
-      <c r="I85" s="21"/>
+      <c r="A85" s="33"/>
+      <c r="B85" s="33"/>
+      <c r="C85" s="34"/>
+      <c r="D85" s="34"/>
+      <c r="E85" s="33"/>
+      <c r="F85" s="35"/>
+      <c r="G85" s="33"/>
+      <c r="H85" s="36"/>
+      <c r="I85" s="37"/>
     </row>
     <row r="86" spans="1:9">
-      <c r="A86" s="9"/>
-      <c r="B86" s="9"/>
-      <c r="C86" s="9"/>
-      <c r="D86" s="9"/>
-      <c r="E86" s="10"/>
-      <c r="F86" s="9"/>
-      <c r="G86" s="9"/>
-      <c r="H86" s="11"/>
-      <c r="I86" s="21"/>
+      <c r="A86" s="33"/>
+      <c r="B86" s="33"/>
+      <c r="C86" s="34"/>
+      <c r="D86" s="34"/>
+      <c r="E86" s="33"/>
+      <c r="F86" s="35"/>
+      <c r="G86" s="33"/>
+      <c r="H86" s="36"/>
+      <c r="I86" s="37"/>
     </row>
     <row r="87" spans="1:9">
-      <c r="A87" s="9"/>
-      <c r="B87" s="9"/>
-      <c r="C87" s="9"/>
-      <c r="D87" s="9"/>
-      <c r="E87" s="10"/>
-      <c r="F87" s="9"/>
-      <c r="G87" s="9"/>
-      <c r="H87" s="11"/>
-      <c r="I87" s="21"/>
+      <c r="A87" s="33"/>
+      <c r="B87" s="33"/>
+      <c r="C87" s="34"/>
+      <c r="D87" s="34"/>
+      <c r="E87" s="33"/>
+      <c r="F87" s="35"/>
+      <c r="G87" s="33"/>
+      <c r="H87" s="36"/>
+      <c r="I87" s="37"/>
     </row>
     <row r="88" spans="1:9">
-      <c r="A88" s="9"/>
-      <c r="B88" s="9"/>
-      <c r="C88" s="9"/>
-      <c r="D88" s="9"/>
-      <c r="E88" s="10"/>
-      <c r="F88" s="9"/>
-      <c r="G88" s="9"/>
-      <c r="H88" s="11"/>
-      <c r="I88" s="21"/>
+      <c r="A88" s="33"/>
+      <c r="B88" s="33"/>
+      <c r="C88" s="34"/>
+      <c r="D88" s="34"/>
+      <c r="E88" s="33"/>
+      <c r="F88" s="35"/>
+      <c r="G88" s="33"/>
+      <c r="H88" s="36"/>
+      <c r="I88" s="37"/>
     </row>
     <row r="89" spans="1:9">
-      <c r="A89" s="9"/>
-      <c r="B89" s="9"/>
-      <c r="C89" s="9"/>
-      <c r="D89" s="9"/>
-      <c r="E89" s="10"/>
-      <c r="F89" s="9"/>
-      <c r="G89" s="9"/>
-      <c r="H89" s="11"/>
-      <c r="I89" s="21"/>
+      <c r="A89" s="33"/>
+      <c r="B89" s="33"/>
+      <c r="C89" s="34"/>
+      <c r="D89" s="34"/>
+      <c r="E89" s="33"/>
+      <c r="F89" s="35"/>
+      <c r="G89" s="33"/>
+      <c r="H89" s="36"/>
+      <c r="I89" s="37"/>
     </row>
     <row r="90" spans="1:9">
-      <c r="A90" s="9"/>
-      <c r="B90" s="9"/>
-      <c r="C90" s="9"/>
-      <c r="D90" s="9"/>
-      <c r="E90" s="10"/>
-      <c r="F90" s="9"/>
-      <c r="G90" s="9"/>
-      <c r="H90" s="11"/>
-      <c r="I90" s="21"/>
+      <c r="A90" s="33"/>
+      <c r="B90" s="33"/>
+      <c r="C90" s="34"/>
+      <c r="D90" s="34"/>
+      <c r="E90" s="33"/>
+      <c r="F90" s="35"/>
+      <c r="G90" s="33"/>
+      <c r="H90" s="36"/>
+      <c r="I90" s="37"/>
     </row>
     <row r="91" spans="1:9">
-      <c r="A91" s="9"/>
-      <c r="B91" s="9"/>
-      <c r="C91" s="9"/>
-      <c r="D91" s="9"/>
-      <c r="E91" s="10"/>
-      <c r="F91" s="9"/>
-      <c r="G91" s="9"/>
-      <c r="H91" s="11"/>
-      <c r="I91" s="21"/>
+      <c r="A91" s="33"/>
+      <c r="B91" s="33"/>
+      <c r="C91" s="34"/>
+      <c r="D91" s="34"/>
+      <c r="E91" s="33"/>
+      <c r="F91" s="35"/>
+      <c r="G91" s="33"/>
+      <c r="H91" s="36"/>
+      <c r="I91" s="37"/>
     </row>
     <row r="92" spans="1:9">
-      <c r="A92" s="9"/>
-      <c r="B92" s="9"/>
-      <c r="C92" s="9"/>
-      <c r="D92" s="9"/>
-      <c r="E92" s="10"/>
-      <c r="F92" s="9"/>
-      <c r="G92" s="9"/>
-      <c r="H92" s="11"/>
-      <c r="I92" s="21"/>
+      <c r="A92" s="33"/>
+      <c r="B92" s="33"/>
+      <c r="C92" s="34"/>
+      <c r="D92" s="34"/>
+      <c r="E92" s="33"/>
+      <c r="F92" s="35"/>
+      <c r="G92" s="33"/>
+      <c r="H92" s="36"/>
+      <c r="I92" s="37"/>
     </row>
     <row r="93" spans="1:9">
-      <c r="A93" s="9"/>
-      <c r="B93" s="9"/>
-      <c r="C93" s="9"/>
-      <c r="D93" s="9"/>
-      <c r="E93" s="10"/>
-      <c r="F93" s="9"/>
-      <c r="G93" s="9"/>
-      <c r="H93" s="11"/>
-      <c r="I93" s="21"/>
+      <c r="A93" s="33"/>
+      <c r="B93" s="33"/>
+      <c r="C93" s="34"/>
+      <c r="D93" s="34"/>
+      <c r="E93" s="33"/>
+      <c r="F93" s="35"/>
+      <c r="G93" s="33"/>
+      <c r="H93" s="36"/>
+      <c r="I93" s="37"/>
     </row>
     <row r="94" spans="1:9">
-      <c r="A94" s="9"/>
-      <c r="B94" s="9"/>
-      <c r="C94" s="9"/>
-      <c r="D94" s="9"/>
-      <c r="E94" s="10"/>
-      <c r="F94" s="9"/>
-      <c r="G94" s="9"/>
-      <c r="H94" s="11"/>
-      <c r="I94" s="21"/>
+      <c r="A94" s="33"/>
+      <c r="B94" s="33"/>
+      <c r="C94" s="34"/>
+      <c r="D94" s="34"/>
+      <c r="E94" s="33"/>
+      <c r="F94" s="35"/>
+      <c r="G94" s="33"/>
+      <c r="H94" s="36"/>
+      <c r="I94" s="37"/>
     </row>
     <row r="95" spans="1:9">
-      <c r="A95" s="9"/>
-      <c r="B95" s="9"/>
-      <c r="C95" s="9"/>
-      <c r="D95" s="9"/>
-      <c r="E95" s="10"/>
-      <c r="F95" s="9"/>
-      <c r="G95" s="9"/>
-      <c r="H95" s="11"/>
-      <c r="I95" s="21"/>
+      <c r="A95" s="33"/>
+      <c r="B95" s="33"/>
+      <c r="C95" s="34"/>
+      <c r="D95" s="34"/>
+      <c r="E95" s="33"/>
+      <c r="F95" s="35"/>
+      <c r="G95" s="33"/>
+      <c r="H95" s="36"/>
+      <c r="I95" s="37"/>
     </row>
     <row r="96" spans="1:9">
-      <c r="A96" s="9"/>
-      <c r="B96" s="9"/>
-      <c r="C96" s="9"/>
-      <c r="D96" s="9"/>
-      <c r="E96" s="10"/>
-      <c r="F96" s="9"/>
-      <c r="G96" s="9"/>
-      <c r="H96" s="11"/>
-      <c r="I96" s="21"/>
+      <c r="A96" s="33"/>
+      <c r="B96" s="33"/>
+      <c r="C96" s="34"/>
+      <c r="D96" s="34"/>
+      <c r="E96" s="33"/>
+      <c r="F96" s="35"/>
+      <c r="G96" s="33"/>
+      <c r="H96" s="36"/>
+      <c r="I96" s="37"/>
     </row>
     <row r="97" spans="1:9">
-      <c r="A97" s="9"/>
-      <c r="B97" s="9"/>
-      <c r="C97" s="9"/>
-      <c r="D97" s="9"/>
-      <c r="E97" s="10"/>
-      <c r="F97" s="9"/>
-      <c r="G97" s="9"/>
-      <c r="H97" s="11"/>
-      <c r="I97" s="21"/>
+      <c r="A97" s="33"/>
+      <c r="B97" s="33"/>
+      <c r="C97" s="34"/>
+      <c r="D97" s="34"/>
+      <c r="E97" s="33"/>
+      <c r="F97" s="35"/>
+      <c r="G97" s="33"/>
+      <c r="H97" s="36"/>
+      <c r="I97" s="37"/>
     </row>
     <row r="98" spans="1:9">
-      <c r="A98" s="9"/>
-      <c r="B98" s="9"/>
-      <c r="C98" s="9"/>
-      <c r="D98" s="9"/>
-      <c r="E98" s="10"/>
-      <c r="F98" s="9"/>
-      <c r="G98" s="9"/>
-      <c r="H98" s="11"/>
-      <c r="I98" s="21"/>
+      <c r="A98" s="33"/>
+      <c r="B98" s="33"/>
+      <c r="C98" s="34"/>
+      <c r="D98" s="34"/>
+      <c r="E98" s="33"/>
+      <c r="F98" s="35"/>
+      <c r="G98" s="33"/>
+      <c r="H98" s="36"/>
+      <c r="I98" s="37"/>
     </row>
     <row r="99" spans="1:9">
-      <c r="A99" s="9"/>
-      <c r="B99" s="9"/>
-      <c r="C99" s="9"/>
-      <c r="D99" s="9"/>
-      <c r="E99" s="10"/>
-      <c r="F99" s="9"/>
-      <c r="G99" s="9"/>
-      <c r="H99" s="11"/>
-      <c r="I99" s="21"/>
+      <c r="A99" s="33"/>
+      <c r="B99" s="33"/>
+      <c r="C99" s="34"/>
+      <c r="D99" s="34"/>
+      <c r="E99" s="33"/>
+      <c r="F99" s="35"/>
+      <c r="G99" s="33"/>
+      <c r="H99" s="36"/>
+      <c r="I99" s="37"/>
     </row>
     <row r="100" spans="1:9">
-      <c r="A100" s="9"/>
-      <c r="B100" s="9"/>
-      <c r="C100" s="9"/>
-      <c r="D100" s="9"/>
-      <c r="E100" s="10"/>
-      <c r="F100" s="9"/>
-      <c r="G100" s="9"/>
-      <c r="H100" s="11"/>
-      <c r="I100" s="21"/>
+      <c r="A100" s="33"/>
+      <c r="B100" s="33"/>
+      <c r="C100" s="34"/>
+      <c r="D100" s="34"/>
+      <c r="E100" s="33"/>
+      <c r="F100" s="35"/>
+      <c r="G100" s="33"/>
+      <c r="H100" s="36"/>
+      <c r="I100" s="37"/>
     </row>
     <row r="101" spans="1:9">
-      <c r="A101" s="9"/>
-      <c r="B101" s="9"/>
-      <c r="C101" s="9"/>
-      <c r="D101" s="9"/>
-      <c r="E101" s="10"/>
-      <c r="F101" s="9"/>
-      <c r="G101" s="9"/>
-      <c r="H101" s="11"/>
-      <c r="I101" s="21"/>
+      <c r="A101" s="38"/>
+      <c r="B101" s="38"/>
+      <c r="C101" s="39"/>
+      <c r="D101" s="39"/>
+      <c r="E101" s="38"/>
+      <c r="F101" s="40"/>
+      <c r="G101" s="38"/>
+      <c r="H101" s="41"/>
+      <c r="I101" s="42"/>
     </row>
     <row r="102" spans="1:9">
       <c r="A102" s="9"/>
@@ -2144,7 +2201,7 @@
       <c r="F102" s="9"/>
       <c r="G102" s="9"/>
       <c r="H102" s="11"/>
-      <c r="I102" s="21"/>
+      <c r="I102" s="20"/>
     </row>
     <row r="103" spans="1:9">
       <c r="A103" s="9"/>
@@ -2155,7 +2212,7 @@
       <c r="F103" s="9"/>
       <c r="G103" s="9"/>
       <c r="H103" s="11"/>
-      <c r="I103" s="21"/>
+      <c r="I103" s="20"/>
     </row>
     <row r="104" spans="1:9">
       <c r="A104" s="9"/>
@@ -2166,7 +2223,7 @@
       <c r="F104" s="9"/>
       <c r="G104" s="9"/>
       <c r="H104" s="11"/>
-      <c r="I104" s="21"/>
+      <c r="I104" s="20"/>
     </row>
     <row r="105" spans="1:9">
       <c r="A105" s="9"/>
@@ -2177,7 +2234,7 @@
       <c r="F105" s="9"/>
       <c r="G105" s="9"/>
       <c r="H105" s="11"/>
-      <c r="I105" s="21"/>
+      <c r="I105" s="20"/>
     </row>
     <row r="106" spans="1:9">
       <c r="A106" s="9"/>
@@ -2188,7 +2245,7 @@
       <c r="F106" s="9"/>
       <c r="G106" s="9"/>
       <c r="H106" s="11"/>
-      <c r="I106" s="21"/>
+      <c r="I106" s="20"/>
     </row>
     <row r="107" spans="1:9">
       <c r="A107" s="9"/>
@@ -2199,7 +2256,7 @@
       <c r="F107" s="9"/>
       <c r="G107" s="9"/>
       <c r="H107" s="11"/>
-      <c r="I107" s="21"/>
+      <c r="I107" s="20"/>
     </row>
     <row r="108" spans="1:9">
       <c r="A108" s="9"/>
@@ -2210,7 +2267,7 @@
       <c r="F108" s="9"/>
       <c r="G108" s="9"/>
       <c r="H108" s="11"/>
-      <c r="I108" s="21"/>
+      <c r="I108" s="20"/>
     </row>
     <row r="109" spans="1:9">
       <c r="A109" s="9"/>
@@ -2221,7 +2278,7 @@
       <c r="F109" s="9"/>
       <c r="G109" s="9"/>
       <c r="H109" s="11"/>
-      <c r="I109" s="21"/>
+      <c r="I109" s="20"/>
     </row>
     <row r="110" spans="1:9">
       <c r="A110" s="9"/>
@@ -2232,7 +2289,7 @@
       <c r="F110" s="9"/>
       <c r="G110" s="9"/>
       <c r="H110" s="11"/>
-      <c r="I110" s="21"/>
+      <c r="I110" s="20"/>
     </row>
     <row r="111" spans="1:9">
       <c r="A111" s="9"/>
@@ -2243,7 +2300,7 @@
       <c r="F111" s="9"/>
       <c r="G111" s="9"/>
       <c r="H111" s="11"/>
-      <c r="I111" s="21"/>
+      <c r="I111" s="20"/>
     </row>
     <row r="112" spans="1:9">
       <c r="A112" s="9"/>
@@ -2254,7 +2311,7 @@
       <c r="F112" s="9"/>
       <c r="G112" s="9"/>
       <c r="H112" s="11"/>
-      <c r="I112" s="21"/>
+      <c r="I112" s="20"/>
     </row>
     <row r="113" spans="1:9">
       <c r="A113" s="9"/>
@@ -2265,7 +2322,7 @@
       <c r="F113" s="9"/>
       <c r="G113" s="9"/>
       <c r="H113" s="11"/>
-      <c r="I113" s="21"/>
+      <c r="I113" s="20"/>
     </row>
     <row r="114" spans="1:9">
       <c r="A114" s="9"/>
@@ -2276,7 +2333,7 @@
       <c r="F114" s="9"/>
       <c r="G114" s="9"/>
       <c r="H114" s="11"/>
-      <c r="I114" s="21"/>
+      <c r="I114" s="20"/>
     </row>
     <row r="115" spans="1:9">
       <c r="A115" s="9"/>
@@ -2287,7 +2344,7 @@
       <c r="F115" s="9"/>
       <c r="G115" s="9"/>
       <c r="H115" s="11"/>
-      <c r="I115" s="21"/>
+      <c r="I115" s="20"/>
     </row>
     <row r="116" spans="1:9">
       <c r="A116" s="9"/>
@@ -2298,7 +2355,7 @@
       <c r="F116" s="9"/>
       <c r="G116" s="9"/>
       <c r="H116" s="11"/>
-      <c r="I116" s="21"/>
+      <c r="I116" s="20"/>
     </row>
     <row r="117" spans="1:9">
       <c r="A117" s="9"/>
@@ -2309,7 +2366,7 @@
       <c r="F117" s="9"/>
       <c r="G117" s="9"/>
       <c r="H117" s="11"/>
-      <c r="I117" s="21"/>
+      <c r="I117" s="20"/>
     </row>
     <row r="118" spans="1:9">
       <c r="A118" s="9"/>
@@ -2320,7 +2377,7 @@
       <c r="F118" s="9"/>
       <c r="G118" s="9"/>
       <c r="H118" s="11"/>
-      <c r="I118" s="21"/>
+      <c r="I118" s="20"/>
     </row>
     <row r="119" spans="1:9">
       <c r="A119" s="9"/>
@@ -2331,7 +2388,7 @@
       <c r="F119" s="9"/>
       <c r="G119" s="9"/>
       <c r="H119" s="11"/>
-      <c r="I119" s="21"/>
+      <c r="I119" s="20"/>
     </row>
     <row r="120" spans="1:9">
       <c r="A120" s="9"/>
@@ -2342,7 +2399,7 @@
       <c r="F120" s="9"/>
       <c r="G120" s="9"/>
       <c r="H120" s="11"/>
-      <c r="I120" s="21"/>
+      <c r="I120" s="20"/>
     </row>
     <row r="121" spans="1:9">
       <c r="A121" s="9"/>
@@ -2353,7 +2410,7 @@
       <c r="F121" s="9"/>
       <c r="G121" s="9"/>
       <c r="H121" s="11"/>
-      <c r="I121" s="21"/>
+      <c r="I121" s="20"/>
     </row>
     <row r="122" spans="1:9">
       <c r="A122" s="9"/>
@@ -2364,7 +2421,7 @@
       <c r="F122" s="9"/>
       <c r="G122" s="9"/>
       <c r="H122" s="11"/>
-      <c r="I122" s="21"/>
+      <c r="I122" s="20"/>
     </row>
     <row r="123" spans="1:9">
       <c r="A123" s="9"/>
@@ -2375,7 +2432,7 @@
       <c r="F123" s="9"/>
       <c r="G123" s="9"/>
       <c r="H123" s="11"/>
-      <c r="I123" s="21"/>
+      <c r="I123" s="20"/>
     </row>
     <row r="124" spans="1:9">
       <c r="A124" s="9"/>
@@ -2386,7 +2443,7 @@
       <c r="F124" s="9"/>
       <c r="G124" s="9"/>
       <c r="H124" s="11"/>
-      <c r="I124" s="21"/>
+      <c r="I124" s="20"/>
     </row>
     <row r="125" spans="1:9">
       <c r="A125" s="9"/>
@@ -2397,7 +2454,7 @@
       <c r="F125" s="9"/>
       <c r="G125" s="9"/>
       <c r="H125" s="11"/>
-      <c r="I125" s="21"/>
+      <c r="I125" s="20"/>
     </row>
     <row r="126" spans="1:9">
       <c r="A126" s="9"/>
@@ -2408,7 +2465,7 @@
       <c r="F126" s="9"/>
       <c r="G126" s="9"/>
       <c r="H126" s="11"/>
-      <c r="I126" s="21"/>
+      <c r="I126" s="20"/>
     </row>
     <row r="127" spans="1:9">
       <c r="A127" s="9"/>
@@ -2419,7 +2476,7 @@
       <c r="F127" s="9"/>
       <c r="G127" s="9"/>
       <c r="H127" s="11"/>
-      <c r="I127" s="21"/>
+      <c r="I127" s="20"/>
     </row>
     <row r="128" spans="1:9">
       <c r="A128" s="9"/>
@@ -2430,7 +2487,7 @@
       <c r="F128" s="9"/>
       <c r="G128" s="9"/>
       <c r="H128" s="11"/>
-      <c r="I128" s="21"/>
+      <c r="I128" s="20"/>
     </row>
     <row r="129" spans="1:9">
       <c r="A129" s="9"/>
@@ -2441,7 +2498,7 @@
       <c r="F129" s="9"/>
       <c r="G129" s="9"/>
       <c r="H129" s="11"/>
-      <c r="I129" s="21"/>
+      <c r="I129" s="20"/>
     </row>
     <row r="130" spans="1:9">
       <c r="A130" s="9"/>
@@ -2452,7 +2509,7 @@
       <c r="F130" s="9"/>
       <c r="G130" s="9"/>
       <c r="H130" s="11"/>
-      <c r="I130" s="21"/>
+      <c r="I130" s="20"/>
     </row>
     <row r="131" spans="1:9">
       <c r="A131" s="9"/>
@@ -2463,7 +2520,7 @@
       <c r="F131" s="9"/>
       <c r="G131" s="9"/>
       <c r="H131" s="11"/>
-      <c r="I131" s="21"/>
+      <c r="I131" s="20"/>
     </row>
     <row r="132" spans="1:9">
       <c r="A132" s="9"/>
@@ -2474,7 +2531,7 @@
       <c r="F132" s="9"/>
       <c r="G132" s="9"/>
       <c r="H132" s="11"/>
-      <c r="I132" s="21"/>
+      <c r="I132" s="20"/>
     </row>
     <row r="133" spans="1:9">
       <c r="A133" s="9"/>
@@ -2485,7 +2542,7 @@
       <c r="F133" s="9"/>
       <c r="G133" s="9"/>
       <c r="H133" s="11"/>
-      <c r="I133" s="21"/>
+      <c r="I133" s="20"/>
     </row>
     <row r="134" spans="1:9">
       <c r="A134" s="9"/>
@@ -2496,7 +2553,7 @@
       <c r="F134" s="9"/>
       <c r="G134" s="9"/>
       <c r="H134" s="11"/>
-      <c r="I134" s="21"/>
+      <c r="I134" s="20"/>
     </row>
     <row r="135" spans="1:9">
       <c r="A135" s="9"/>
@@ -2507,7 +2564,7 @@
       <c r="F135" s="9"/>
       <c r="G135" s="9"/>
       <c r="H135" s="11"/>
-      <c r="I135" s="21"/>
+      <c r="I135" s="20"/>
     </row>
     <row r="136" spans="1:9">
       <c r="A136" s="9"/>
@@ -2518,7 +2575,7 @@
       <c r="F136" s="9"/>
       <c r="G136" s="9"/>
       <c r="H136" s="11"/>
-      <c r="I136" s="21"/>
+      <c r="I136" s="20"/>
     </row>
     <row r="137" spans="1:9">
       <c r="A137" s="9"/>
@@ -2529,7 +2586,7 @@
       <c r="F137" s="9"/>
       <c r="G137" s="9"/>
       <c r="H137" s="11"/>
-      <c r="I137" s="21"/>
+      <c r="I137" s="20"/>
     </row>
     <row r="138" spans="1:9">
       <c r="A138" s="9"/>
@@ -2540,7 +2597,7 @@
       <c r="F138" s="9"/>
       <c r="G138" s="9"/>
       <c r="H138" s="11"/>
-      <c r="I138" s="21"/>
+      <c r="I138" s="20"/>
     </row>
     <row r="139" spans="1:9">
       <c r="A139" s="9"/>
@@ -2551,7 +2608,7 @@
       <c r="F139" s="9"/>
       <c r="G139" s="9"/>
       <c r="H139" s="11"/>
-      <c r="I139" s="21"/>
+      <c r="I139" s="20"/>
     </row>
     <row r="140" spans="1:9">
       <c r="A140" s="9"/>
@@ -2562,7 +2619,7 @@
       <c r="F140" s="9"/>
       <c r="G140" s="9"/>
       <c r="H140" s="11"/>
-      <c r="I140" s="21"/>
+      <c r="I140" s="20"/>
     </row>
     <row r="141" spans="1:9">
       <c r="A141" s="9"/>
@@ -2573,7 +2630,7 @@
       <c r="F141" s="9"/>
       <c r="G141" s="9"/>
       <c r="H141" s="11"/>
-      <c r="I141" s="21"/>
+      <c r="I141" s="20"/>
     </row>
     <row r="142" spans="1:9">
       <c r="A142" s="9"/>
@@ -2584,7 +2641,7 @@
       <c r="F142" s="9"/>
       <c r="G142" s="9"/>
       <c r="H142" s="11"/>
-      <c r="I142" s="21"/>
+      <c r="I142" s="20"/>
     </row>
     <row r="143" spans="1:9">
       <c r="A143" s="9"/>
@@ -2595,7 +2652,7 @@
       <c r="F143" s="9"/>
       <c r="G143" s="9"/>
       <c r="H143" s="11"/>
-      <c r="I143" s="21"/>
+      <c r="I143" s="20"/>
     </row>
     <row r="144" spans="1:9">
       <c r="A144" s="9"/>
@@ -2606,7 +2663,7 @@
       <c r="F144" s="9"/>
       <c r="G144" s="9"/>
       <c r="H144" s="11"/>
-      <c r="I144" s="21"/>
+      <c r="I144" s="20"/>
     </row>
     <row r="145" spans="1:9">
       <c r="A145" s="9"/>
@@ -2617,7 +2674,7 @@
       <c r="F145" s="9"/>
       <c r="G145" s="9"/>
       <c r="H145" s="11"/>
-      <c r="I145" s="21"/>
+      <c r="I145" s="20"/>
     </row>
     <row r="146" spans="1:9">
       <c r="A146" s="9"/>
@@ -2628,7 +2685,7 @@
       <c r="F146" s="9"/>
       <c r="G146" s="9"/>
       <c r="H146" s="11"/>
-      <c r="I146" s="21"/>
+      <c r="I146" s="20"/>
     </row>
     <row r="147" spans="1:9">
       <c r="A147" s="9"/>
@@ -2639,7 +2696,7 @@
       <c r="F147" s="9"/>
       <c r="G147" s="9"/>
       <c r="H147" s="11"/>
-      <c r="I147" s="21"/>
+      <c r="I147" s="20"/>
     </row>
     <row r="148" spans="1:9">
       <c r="A148" s="9"/>
@@ -2650,7 +2707,7 @@
       <c r="F148" s="9"/>
       <c r="G148" s="9"/>
       <c r="H148" s="11"/>
-      <c r="I148" s="21"/>
+      <c r="I148" s="20"/>
     </row>
     <row r="149" spans="1:9">
       <c r="A149" s="9"/>
@@ -2661,7 +2718,7 @@
       <c r="F149" s="9"/>
       <c r="G149" s="9"/>
       <c r="H149" s="11"/>
-      <c r="I149" s="21"/>
+      <c r="I149" s="20"/>
     </row>
     <row r="150" spans="1:9">
       <c r="A150" s="9"/>
@@ -2672,7 +2729,7 @@
       <c r="F150" s="9"/>
       <c r="G150" s="9"/>
       <c r="H150" s="11"/>
-      <c r="I150" s="21"/>
+      <c r="I150" s="20"/>
     </row>
     <row r="151" spans="1:9">
       <c r="A151" s="9"/>
@@ -2683,7 +2740,7 @@
       <c r="F151" s="9"/>
       <c r="G151" s="9"/>
       <c r="H151" s="11"/>
-      <c r="I151" s="21"/>
+      <c r="I151" s="20"/>
     </row>
     <row r="152" spans="1:9">
       <c r="A152" s="9"/>
@@ -2694,7 +2751,7 @@
       <c r="F152" s="9"/>
       <c r="G152" s="9"/>
       <c r="H152" s="11"/>
-      <c r="I152" s="21"/>
+      <c r="I152" s="20"/>
     </row>
     <row r="153" spans="1:9">
       <c r="A153" s="9"/>
@@ -2705,7 +2762,7 @@
       <c r="F153" s="9"/>
       <c r="G153" s="9"/>
       <c r="H153" s="11"/>
-      <c r="I153" s="21"/>
+      <c r="I153" s="20"/>
     </row>
     <row r="154" spans="1:9">
       <c r="A154" s="9"/>
@@ -2716,7 +2773,7 @@
       <c r="F154" s="9"/>
       <c r="G154" s="9"/>
       <c r="H154" s="11"/>
-      <c r="I154" s="21"/>
+      <c r="I154" s="20"/>
     </row>
     <row r="155" spans="1:9">
       <c r="A155" s="9"/>
@@ -2727,7 +2784,7 @@
       <c r="F155" s="9"/>
       <c r="G155" s="9"/>
       <c r="H155" s="11"/>
-      <c r="I155" s="21"/>
+      <c r="I155" s="20"/>
     </row>
     <row r="156" spans="1:9">
       <c r="A156" s="9"/>
@@ -2738,7 +2795,7 @@
       <c r="F156" s="9"/>
       <c r="G156" s="9"/>
       <c r="H156" s="11"/>
-      <c r="I156" s="21"/>
+      <c r="I156" s="20"/>
     </row>
     <row r="157" spans="1:9">
       <c r="A157" s="9"/>
@@ -2749,7 +2806,7 @@
       <c r="F157" s="9"/>
       <c r="G157" s="9"/>
       <c r="H157" s="11"/>
-      <c r="I157" s="21"/>
+      <c r="I157" s="20"/>
     </row>
     <row r="158" spans="1:9">
       <c r="A158" s="9"/>
@@ -2760,7 +2817,7 @@
       <c r="F158" s="9"/>
       <c r="G158" s="9"/>
       <c r="H158" s="11"/>
-      <c r="I158" s="21"/>
+      <c r="I158" s="20"/>
     </row>
     <row r="159" spans="1:9">
       <c r="A159" s="9"/>
@@ -2771,7 +2828,7 @@
       <c r="F159" s="9"/>
       <c r="G159" s="9"/>
       <c r="H159" s="11"/>
-      <c r="I159" s="21"/>
+      <c r="I159" s="20"/>
     </row>
     <row r="160" spans="1:9">
       <c r="A160" s="9"/>
@@ -2782,7 +2839,7 @@
       <c r="F160" s="9"/>
       <c r="G160" s="9"/>
       <c r="H160" s="11"/>
-      <c r="I160" s="21"/>
+      <c r="I160" s="20"/>
     </row>
     <row r="161" spans="1:9">
       <c r="A161" s="9"/>
@@ -2793,7 +2850,7 @@
       <c r="F161" s="9"/>
       <c r="G161" s="9"/>
       <c r="H161" s="11"/>
-      <c r="I161" s="21"/>
+      <c r="I161" s="20"/>
     </row>
     <row r="162" spans="1:9">
       <c r="A162" s="9"/>
@@ -2804,7 +2861,7 @@
       <c r="F162" s="9"/>
       <c r="G162" s="9"/>
       <c r="H162" s="11"/>
-      <c r="I162" s="21"/>
+      <c r="I162" s="20"/>
     </row>
     <row r="163" spans="1:9">
       <c r="A163" s="9"/>
@@ -2815,7 +2872,7 @@
       <c r="F163" s="9"/>
       <c r="G163" s="9"/>
       <c r="H163" s="11"/>
-      <c r="I163" s="21"/>
+      <c r="I163" s="20"/>
     </row>
     <row r="164" spans="1:9">
       <c r="A164" s="9"/>
@@ -2826,7 +2883,7 @@
       <c r="F164" s="9"/>
       <c r="G164" s="9"/>
       <c r="H164" s="11"/>
-      <c r="I164" s="21"/>
+      <c r="I164" s="20"/>
     </row>
     <row r="165" spans="1:9">
       <c r="A165" s="9"/>
@@ -2837,7 +2894,7 @@
       <c r="F165" s="9"/>
       <c r="G165" s="9"/>
       <c r="H165" s="11"/>
-      <c r="I165" s="21"/>
+      <c r="I165" s="20"/>
     </row>
     <row r="166" spans="1:9">
       <c r="A166" s="9"/>
@@ -2848,7 +2905,7 @@
       <c r="F166" s="9"/>
       <c r="G166" s="9"/>
       <c r="H166" s="11"/>
-      <c r="I166" s="21"/>
+      <c r="I166" s="20"/>
     </row>
     <row r="167" spans="1:9">
       <c r="A167" s="9"/>
@@ -2859,7 +2916,7 @@
       <c r="F167" s="9"/>
       <c r="G167" s="9"/>
       <c r="H167" s="11"/>
-      <c r="I167" s="21"/>
+      <c r="I167" s="20"/>
     </row>
     <row r="168" spans="1:9">
       <c r="A168" s="9"/>
@@ -2870,7 +2927,7 @@
       <c r="F168" s="9"/>
       <c r="G168" s="9"/>
       <c r="H168" s="11"/>
-      <c r="I168" s="21"/>
+      <c r="I168" s="20"/>
     </row>
     <row r="169" spans="1:9">
       <c r="A169" s="9"/>
@@ -2881,7 +2938,7 @@
       <c r="F169" s="9"/>
       <c r="G169" s="9"/>
       <c r="H169" s="11"/>
-      <c r="I169" s="21"/>
+      <c r="I169" s="20"/>
     </row>
     <row r="170" spans="1:9">
       <c r="A170" s="9"/>
@@ -2892,7 +2949,7 @@
       <c r="F170" s="9"/>
       <c r="G170" s="9"/>
       <c r="H170" s="11"/>
-      <c r="I170" s="21"/>
+      <c r="I170" s="20"/>
     </row>
     <row r="171" spans="1:9">
       <c r="A171" s="9"/>
@@ -2903,7 +2960,7 @@
       <c r="F171" s="9"/>
       <c r="G171" s="9"/>
       <c r="H171" s="11"/>
-      <c r="I171" s="21"/>
+      <c r="I171" s="20"/>
     </row>
     <row r="172" spans="1:9">
       <c r="A172" s="9"/>
@@ -2914,7 +2971,7 @@
       <c r="F172" s="9"/>
       <c r="G172" s="9"/>
       <c r="H172" s="11"/>
-      <c r="I172" s="21"/>
+      <c r="I172" s="20"/>
     </row>
     <row r="173" spans="1:9">
       <c r="A173" s="9"/>
@@ -2925,7 +2982,7 @@
       <c r="F173" s="9"/>
       <c r="G173" s="9"/>
       <c r="H173" s="11"/>
-      <c r="I173" s="21"/>
+      <c r="I173" s="20"/>
     </row>
     <row r="174" spans="1:9">
       <c r="A174" s="9"/>
@@ -2936,7 +2993,7 @@
       <c r="F174" s="9"/>
       <c r="G174" s="9"/>
       <c r="H174" s="11"/>
-      <c r="I174" s="21"/>
+      <c r="I174" s="20"/>
     </row>
     <row r="175" spans="1:9">
       <c r="A175" s="9"/>
@@ -2947,7 +3004,7 @@
       <c r="F175" s="9"/>
       <c r="G175" s="9"/>
       <c r="H175" s="11"/>
-      <c r="I175" s="21"/>
+      <c r="I175" s="20"/>
     </row>
     <row r="176" spans="1:9">
       <c r="A176" s="9"/>
@@ -2958,7 +3015,7 @@
       <c r="F176" s="9"/>
       <c r="G176" s="9"/>
       <c r="H176" s="11"/>
-      <c r="I176" s="21"/>
+      <c r="I176" s="20"/>
     </row>
     <row r="177" spans="1:9">
       <c r="A177" s="9"/>
@@ -2969,7 +3026,7 @@
       <c r="F177" s="9"/>
       <c r="G177" s="9"/>
       <c r="H177" s="11"/>
-      <c r="I177" s="21"/>
+      <c r="I177" s="20"/>
     </row>
     <row r="178" spans="1:9">
       <c r="A178" s="9"/>
@@ -2980,7 +3037,7 @@
       <c r="F178" s="9"/>
       <c r="G178" s="9"/>
       <c r="H178" s="11"/>
-      <c r="I178" s="21"/>
+      <c r="I178" s="20"/>
     </row>
     <row r="179" spans="1:9">
       <c r="A179" s="9"/>
@@ -2991,7 +3048,7 @@
       <c r="F179" s="9"/>
       <c r="G179" s="9"/>
       <c r="H179" s="11"/>
-      <c r="I179" s="21"/>
+      <c r="I179" s="20"/>
     </row>
     <row r="180" spans="1:9">
       <c r="A180" s="9"/>
@@ -3002,7 +3059,7 @@
       <c r="F180" s="9"/>
       <c r="G180" s="9"/>
       <c r="H180" s="11"/>
-      <c r="I180" s="21"/>
+      <c r="I180" s="20"/>
     </row>
     <row r="181" spans="1:9">
       <c r="A181" s="9"/>
@@ -3013,7 +3070,7 @@
       <c r="F181" s="9"/>
       <c r="G181" s="9"/>
       <c r="H181" s="11"/>
-      <c r="I181" s="21"/>
+      <c r="I181" s="20"/>
     </row>
     <row r="182" spans="1:9">
       <c r="A182" s="9"/>
@@ -3024,7 +3081,7 @@
       <c r="F182" s="9"/>
       <c r="G182" s="9"/>
       <c r="H182" s="11"/>
-      <c r="I182" s="21"/>
+      <c r="I182" s="20"/>
     </row>
     <row r="183" spans="1:9">
       <c r="A183" s="9"/>
@@ -3035,7 +3092,7 @@
       <c r="F183" s="9"/>
       <c r="G183" s="9"/>
       <c r="H183" s="11"/>
-      <c r="I183" s="21"/>
+      <c r="I183" s="20"/>
     </row>
     <row r="184" spans="1:9">
       <c r="A184" s="9"/>
@@ -3046,7 +3103,7 @@
       <c r="F184" s="9"/>
       <c r="G184" s="9"/>
       <c r="H184" s="11"/>
-      <c r="I184" s="21"/>
+      <c r="I184" s="20"/>
     </row>
     <row r="185" spans="1:9">
       <c r="A185" s="9"/>
@@ -3057,7 +3114,7 @@
       <c r="F185" s="9"/>
       <c r="G185" s="9"/>
       <c r="H185" s="11"/>
-      <c r="I185" s="21"/>
+      <c r="I185" s="20"/>
     </row>
     <row r="186" spans="1:9">
       <c r="A186" s="9"/>
@@ -3068,7 +3125,7 @@
       <c r="F186" s="9"/>
       <c r="G186" s="9"/>
       <c r="H186" s="11"/>
-      <c r="I186" s="21"/>
+      <c r="I186" s="20"/>
     </row>
     <row r="187" spans="1:9">
       <c r="A187" s="9"/>
@@ -3079,7 +3136,7 @@
       <c r="F187" s="9"/>
       <c r="G187" s="9"/>
       <c r="H187" s="11"/>
-      <c r="I187" s="21"/>
+      <c r="I187" s="20"/>
     </row>
     <row r="188" spans="1:9">
       <c r="A188" s="9"/>
@@ -3090,7 +3147,7 @@
       <c r="F188" s="9"/>
       <c r="G188" s="9"/>
       <c r="H188" s="11"/>
-      <c r="I188" s="21"/>
+      <c r="I188" s="20"/>
     </row>
     <row r="189" spans="1:9">
       <c r="A189" s="9"/>
@@ -3101,7 +3158,7 @@
       <c r="F189" s="9"/>
       <c r="G189" s="9"/>
       <c r="H189" s="11"/>
-      <c r="I189" s="21"/>
+      <c r="I189" s="20"/>
     </row>
     <row r="190" spans="1:9">
       <c r="A190" s="9"/>
@@ -3112,7 +3169,7 @@
       <c r="F190" s="9"/>
       <c r="G190" s="9"/>
       <c r="H190" s="11"/>
-      <c r="I190" s="21"/>
+      <c r="I190" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>